<commit_message>
can read in the csv file
</commit_message>
<xml_diff>
--- a/src/main/java/modules/trackmodel/Track Layout & Vehicle Data vF.xlsx
+++ b/src/main/java/modules/trackmodel/Track Layout & Vehicle Data vF.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="General Information" sheetId="3" r:id="rId1"/>
@@ -1046,8 +1046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L154"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J67" sqref="J67"/>
     </sheetView>
   </sheetViews>
@@ -3977,7 +3977,7 @@
   <dimension ref="A1:L151"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -8581,7 +8581,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="72" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScale="72" workbookViewId="0">
       <selection activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>

</xml_diff>